<commit_message>
Uploaded plan and final workload files
</commit_message>
<xml_diff>
--- a/final-project-workload-final.xlsx
+++ b/final-project-workload-final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markv\Documents\Repositories\computergraphicsassignments\Bachelor\final_project2_ray_tracing\Text\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konto\Documents\ComputerGraphics\projectRepo\template-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AFDF91-285E-4AF5-8579-4412DB7629A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A832B44F-7C70-4449-9873-483A121A1B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2003" yWindow="1792" windowWidth="18299" windowHeight="11866" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workload" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,12 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>FILL IN THE BLUE BOXES ONLY</t>
   </si>
@@ -59,12 +56,6 @@
     <t>member 3</t>
   </si>
   <si>
-    <t>&lt;student id&gt;</t>
-  </si>
-  <si>
-    <t>&lt;student name&gt;</t>
-  </si>
-  <si>
     <t>basic features</t>
   </si>
   <si>
@@ -129,13 +120,22 @@
   </si>
   <si>
     <t>implementation of multisampling</t>
+  </si>
+  <si>
+    <t>Georgios Tsampikos Kontos</t>
+  </si>
+  <si>
+    <t>Davide Tudose</t>
+  </si>
+  <si>
+    <t>Nazar Vasyliev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -188,8 +188,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +211,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9E1F2"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FFD9E1F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -303,10 +320,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,9 +334,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -398,9 +413,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{8611ADE4-4515-4C82-B50F-56F888B4958B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -783,49 +817,49 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:G26"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="48.46484375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="48.46484375" style="31" customWidth="1"/>
-    <col min="4" max="4" width="21.1328125" customWidth="1"/>
-    <col min="5" max="5" width="22.46484375" customWidth="1"/>
-    <col min="6" max="6" width="22.86328125" customWidth="1"/>
-    <col min="7" max="7" width="13.86328125" customWidth="1"/>
-    <col min="8" max="8" width="12.53125" customWidth="1"/>
+    <col min="2" max="2" width="48.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="48.44140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="10.53125" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B2" s="36" t="s">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
-      <c r="C3" s="27"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C3" s="26"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="28"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
@@ -836,422 +870,422 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C5" s="27"/>
+      <c r="D5" s="36">
+        <v>5677416</v>
+      </c>
+      <c r="E5" s="37">
+        <v>5768594</v>
+      </c>
+      <c r="F5" s="38">
+        <v>5887054</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="27"/>
+      <c r="D6" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="23">
         <v>6</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+      <c r="D8" s="9">
+        <v>100</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" ref="G8:G15" si="0">SUM(D8:F8)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="23">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>100</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="24">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <v>100</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="24">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>100</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="25">
+        <v>0.75</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>100</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>100</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="25">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10">
+        <v>100</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="25">
+        <v>1.75</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <v>100</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="24">
-        <v>6</v>
-      </c>
-      <c r="D8" s="10">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10">
-        <v>0</v>
-      </c>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6">
-        <f t="shared" ref="G8:G15" si="0">SUM(D8:F8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="24">
-        <v>1</v>
-      </c>
-      <c r="D9" s="10">
-        <v>0</v>
-      </c>
-      <c r="E9" s="10">
-        <v>0</v>
-      </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="25">
-        <v>1</v>
-      </c>
-      <c r="D10" s="10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="11">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="25">
-        <v>1</v>
-      </c>
-      <c r="D11" s="10">
-        <v>0</v>
-      </c>
-      <c r="E11" s="10">
-        <v>0</v>
-      </c>
-      <c r="F11" s="11">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B12" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="26">
-        <v>0.75</v>
-      </c>
-      <c r="D12" s="10">
-        <v>0</v>
-      </c>
-      <c r="E12" s="10">
-        <v>0</v>
-      </c>
-      <c r="F12" s="11">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="26">
-        <v>1.5</v>
-      </c>
-      <c r="D13" s="10">
-        <v>0</v>
-      </c>
-      <c r="E13" s="10">
-        <v>0</v>
-      </c>
-      <c r="F13" s="11">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B14" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="26">
-        <v>5</v>
-      </c>
-      <c r="D14" s="10">
-        <v>0</v>
-      </c>
-      <c r="E14" s="10">
-        <v>0</v>
-      </c>
-      <c r="F14" s="11">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B15" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="26">
-        <v>1.75</v>
-      </c>
-      <c r="D15" s="10">
-        <v>0</v>
-      </c>
-      <c r="E15" s="10">
-        <v>0</v>
-      </c>
-      <c r="F15" s="11">
-        <v>0</v>
-      </c>
-      <c r="G15" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="30">
+      <c r="C16" s="29">
         <f>SUM(C8:C15)</f>
         <v>18</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="15">
         <f>SUMPRODUCT(C8:C15,D8:D15)/100</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="16">
+        <v>6</v>
+      </c>
+      <c r="E16" s="15">
         <f>SUMPRODUCT($C8:$C15,E8:E15)/100</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="16">
+        <v>6</v>
+      </c>
+      <c r="F16" s="15">
         <f>SUMPRODUCT($C8:$C15,F8:F15)/100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="14"/>
-      <c r="B18" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D19" s="17">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" ref="G19:G24" si="1">SUM(D19:F19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="23">
+        <v>2</v>
+      </c>
+      <c r="D20" s="17">
+        <v>100</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="14"/>
-      <c r="B19" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="24">
+      <c r="C21" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="D21" s="17">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="23">
         <v>1.5</v>
       </c>
-      <c r="D19" s="18">
-        <v>0</v>
-      </c>
-      <c r="E19" s="10">
-        <v>0</v>
-      </c>
-      <c r="F19" s="11">
-        <v>0</v>
-      </c>
-      <c r="G19" s="6">
-        <f t="shared" ref="G19:G24" si="1">SUM(D19:F19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B20" s="9" t="s">
+      <c r="D22" s="17">
+        <v>100</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="24">
-        <v>2</v>
-      </c>
-      <c r="D20" s="18">
-        <v>0</v>
-      </c>
-      <c r="E20" s="10">
-        <v>0</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0</v>
-      </c>
-      <c r="G20" s="6">
+      <c r="C23" s="23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="17">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B21" s="9" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="24">
-        <v>4.5</v>
-      </c>
-      <c r="D21" s="18">
-        <v>0</v>
-      </c>
-      <c r="E21" s="10">
-        <v>0</v>
-      </c>
-      <c r="F21" s="11">
-        <v>0</v>
-      </c>
-      <c r="G21" s="6">
+      <c r="C24" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="D24" s="17">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0</v>
+      </c>
+      <c r="F24" s="10">
+        <v>0</v>
+      </c>
+      <c r="G24" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B22" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="24">
-        <v>1.5</v>
-      </c>
-      <c r="D22" s="18">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10">
-        <v>0</v>
-      </c>
-      <c r="F22" s="11">
-        <v>0</v>
-      </c>
-      <c r="G22" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B23" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="24">
-        <v>1</v>
-      </c>
-      <c r="D23" s="18">
-        <v>0</v>
-      </c>
-      <c r="E23" s="10">
-        <v>0</v>
-      </c>
-      <c r="F23" s="11">
-        <v>0</v>
-      </c>
-      <c r="G23" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B24" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="D24" s="18">
-        <v>0</v>
-      </c>
-      <c r="E24" s="10">
-        <v>0</v>
-      </c>
-      <c r="F24" s="11">
-        <v>0</v>
-      </c>
-      <c r="G24" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B25" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="33">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="32">
         <f>SUM(C19:C24)</f>
         <v>14</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="15">
         <f>SUMPRODUCT($C19:$C24,D19:D24)/100</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="E25" s="15">
         <f>SUMPRODUCT($C19:$C24,E19:E24)/100</f>
         <v>0</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="15">
         <f>SUMPRODUCT($C19:$C24,F19:F24)/100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B26" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="21">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="33"/>
+      <c r="D26" s="20">
         <f>D$16+D25</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="21">
+        <v>9.5</v>
+      </c>
+      <c r="E26" s="20">
         <f>E$16+E25</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="22">
+        <v>6</v>
+      </c>
+      <c r="F26" s="21">
         <f>F$16+F25</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1270,21 +1304,21 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" s="23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" s="23" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>